<commit_message>
MAx growth set up
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BF0151-11B8-4530-BDFB-39A6970663CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A1EE22-E90C-4E4F-B3BD-2D4E75727A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="SRV" sheetId="5" r:id="rId6"/>
     <sheet name="TRA" sheetId="1" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="3" hidden="1">#REF!</definedName>
@@ -171,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="230">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -864,16 +867,35 @@
   <si>
     <t>SRVELC</t>
   </si>
+  <si>
+    <t>DH_IND*</t>
+  </si>
+  <si>
+    <t>DH_SOL*</t>
+  </si>
+  <si>
+    <t>DH_IND</t>
+  </si>
+  <si>
+    <t>DH_SOL</t>
+  </si>
+  <si>
+    <t>SRVSOL</t>
+  </si>
+  <si>
+    <t>SRVLPG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1156,7 +1178,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1258,6 +1280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1655,6 +1678,118 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="Regions"/>
+      <sheetName val="SUP"/>
+      <sheetName val="PWR"/>
+      <sheetName val="RSD"/>
+      <sheetName val="SRV"/>
+      <sheetName val="TRA"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>IE</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>National</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>IE-CW</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>IE-D</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>IE-KE</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>IE-KK</v>
+          </cell>
+          <cell r="I3" t="str">
+            <v>IE-LS</v>
+          </cell>
+          <cell r="J3" t="str">
+            <v>IE-LD</v>
+          </cell>
+          <cell r="K3" t="str">
+            <v>IE-LH</v>
+          </cell>
+          <cell r="L3" t="str">
+            <v>IE-MH</v>
+          </cell>
+          <cell r="M3" t="str">
+            <v>IE-OY</v>
+          </cell>
+          <cell r="N3" t="str">
+            <v>IE-WH</v>
+          </cell>
+          <cell r="O3" t="str">
+            <v>IE-WX</v>
+          </cell>
+          <cell r="P3" t="str">
+            <v>IE-WW</v>
+          </cell>
+          <cell r="Q3" t="str">
+            <v>IE-CE</v>
+          </cell>
+          <cell r="R3" t="str">
+            <v>IE-CO</v>
+          </cell>
+          <cell r="S3" t="str">
+            <v>IE-KY</v>
+          </cell>
+          <cell r="T3" t="str">
+            <v>IE-LK</v>
+          </cell>
+          <cell r="U3" t="str">
+            <v>IE-TA</v>
+          </cell>
+          <cell r="V3" t="str">
+            <v>IE-WD</v>
+          </cell>
+          <cell r="W3" t="str">
+            <v>IE-G</v>
+          </cell>
+          <cell r="X3" t="str">
+            <v>IE-LM</v>
+          </cell>
+          <cell r="Y3" t="str">
+            <v>IE-MO</v>
+          </cell>
+          <cell r="Z3" t="str">
+            <v>IE-RN</v>
+          </cell>
+          <cell r="AA3" t="str">
+            <v>IE-SO</v>
+          </cell>
+          <cell r="AB3" t="str">
+            <v>IE-CN</v>
+          </cell>
+          <cell r="AC3" t="str">
+            <v>IE-DL</v>
+          </cell>
+          <cell r="AD3" t="str">
+            <v>IE-MN</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5801,10 +5936,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N27"/>
+  <dimension ref="A2:N29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5819,7 +5954,7 @@
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
-        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
       <c r="C2" s="2"/>
@@ -5900,7 +6035,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+        <f t="shared" ref="B6:B13" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5916,21 +6051,21 @@
         <v>15</v>
       </c>
       <c r="G6" s="26">
-        <f t="shared" ref="G6:G9" si="1">1+$C14</f>
+        <f t="shared" ref="G6:G13" si="1">1+$C16</f>
         <v>1.05</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
       <c r="I6" s="16">
-        <f t="shared" ref="I6:I11" si="2">-D14</f>
+        <f t="shared" ref="I6:I13" si="2">-D16</f>
         <v>-0.1</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="str">
-        <f t="shared" ref="K6:K11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
+        <f t="shared" ref="K6:K13" si="3">_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
@@ -6044,7 +6179,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f t="shared" ref="B10:B11" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
+        <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_PV</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6060,7 +6195,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="26">
-        <f t="shared" ref="G10:G11" si="5">1+$C18</f>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="H10" s="2">
@@ -6080,7 +6215,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_CSP</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6096,7 +6231,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="H11" s="2">
@@ -6114,40 +6249,84 @@
         <v>PWR maximum growth rate of CSP</v>
       </c>
     </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_PWR_MaxGrowth_DH_IND</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="26">
+        <f t="shared" si="1"/>
+        <v>1.02</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="2"/>
+        <v>-0.1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>PWR maximum growth rate of DH_IND</v>
+      </c>
+    </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_PWR_MaxGrowth_DH_SOL</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="26">
+        <f t="shared" si="1"/>
+        <v>1.02</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="16">
+        <f t="shared" si="2"/>
+        <v>-0.1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>PWR maximum growth rate of DH_SOL</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>117</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D14">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D15">
-        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -6155,10 +6334,10 @@
         <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C16" s="11">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="D16">
         <v>0.1</v>
@@ -6169,13 +6348,13 @@
         <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="C17" s="11">
         <v>0.2</v>
       </c>
       <c r="D17">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -6183,13 +6362,13 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="C18" s="11">
         <v>0.2</v>
       </c>
       <c r="D18">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -6197,7 +6376,7 @@
         <v>128</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C19" s="11">
         <v>0.2</v>
@@ -6206,136 +6385,192 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+    </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="D22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E25" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J25" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="2">
-        <v>2019</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G24" s="26">
-        <f>1+$C29</f>
-        <v>1</v>
-      </c>
-      <c r="H24" s="16">
-        <v>0.6</v>
-      </c>
-      <c r="I24" s="2">
-        <v>3</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2020</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G25" s="26">
-        <f>1+$C30</f>
-        <v>1</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E26">
-        <v>2026</v>
+        <v>154</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2019</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>185</v>
       </c>
       <c r="G26" s="26">
-        <f>1+$C30</f>
+        <f>1+$C31</f>
         <v>1</v>
       </c>
       <c r="H26" s="16">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="I26" s="2">
         <v>3</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="2"/>
-      <c r="E27">
-        <v>2027</v>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2020</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="G27" s="26">
+        <f>1+$C32</f>
+        <v>1</v>
+      </c>
       <c r="H27" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28">
+        <v>2026</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G28" s="26">
+        <f>1+$C32</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="16">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>3</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+      <c r="E29">
+        <v>2027</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H29" s="16">
         <v>2</v>
       </c>
     </row>
@@ -6348,13 +6583,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -6370,7 +6604,7 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
-        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3,Regions!E3:AD3)</f>
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!C3,[1]Regions!E3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="C2" s="2"/>
@@ -6484,7 +6718,7 @@
       </c>
       <c r="J6" s="29">
         <f>1+C26</f>
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
@@ -6524,7 +6758,7 @@
       </c>
       <c r="J7" s="29">
         <f>1+C26</f>
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
@@ -6564,7 +6798,7 @@
       </c>
       <c r="J8" s="29">
         <f>1+C27</f>
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
@@ -6764,7 +6998,7 @@
       </c>
       <c r="J13" s="29">
         <f>1+C30</f>
-        <v>1.1000000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
@@ -6884,14 +7118,14 @@
       </c>
       <c r="J16" s="29">
         <f>1+C33</f>
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
       </c>
       <c r="L16" s="16">
         <f>-D33</f>
-        <v>0.3</v>
+        <v>-0.3</v>
       </c>
       <c r="M16" s="2">
         <v>5</v>
@@ -6923,15 +7157,15 @@
         <v>185</v>
       </c>
       <c r="J17" s="29">
-        <f>1+C33/E33</f>
-        <v>1.1599999999999999</v>
+        <f>1+C33/2</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K17" s="2">
         <v>1</v>
       </c>
       <c r="L17" s="16">
-        <f>-D33</f>
-        <v>0.3</v>
+        <f>-D34</f>
+        <v>-0.1</v>
       </c>
       <c r="M17" s="2">
         <v>5</v>
@@ -6964,7 +7198,7 @@
       </c>
       <c r="J18" s="29">
         <f t="shared" ref="J18:J19" si="1">1+C34</f>
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
@@ -7165,7 +7399,7 @@
         <v>196</v>
       </c>
       <c r="C26" s="11">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -7179,7 +7413,7 @@
         <v>137</v>
       </c>
       <c r="C27" s="11">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -7221,7 +7455,7 @@
         <v>199</v>
       </c>
       <c r="C30" s="11">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="D30">
         <v>0.1</v>
@@ -7263,13 +7497,10 @@
         <v>191</v>
       </c>
       <c r="C33" s="11">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D33">
-        <v>-0.3</v>
-      </c>
-      <c r="E33">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -7280,7 +7511,7 @@
         <v>201</v>
       </c>
       <c r="C34" s="11">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="D34">
         <v>0.1</v>
@@ -7334,11 +7565,11 @@
         <v>7</v>
       </c>
       <c r="F40" s="48" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
       <c r="G40" s="48" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!D$3,"*")</f>
         <v>National</v>
       </c>
       <c r="H40" s="49" t="s">
@@ -7372,10 +7603,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:N24"/>
+  <dimension ref="A2:N28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7394,9 +7625,9 @@
     <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
-        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
       <c r="C2" s="2"/>
@@ -7412,7 +7643,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7429,7 +7660,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7446,7 +7677,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7487,9 +7718,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6:B11" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+        <f t="shared" ref="B6:B11" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
         <v>UC_SRV_MaxGrowth_Biomass</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -7509,25 +7740,25 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f t="shared" ref="J6:J11" si="1">1+C14</f>
-        <v>1.01</v>
+        <f>1+C17</f>
+        <v>1.02</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f t="shared" ref="L6:L11" si="2">-D14</f>
+        <f t="shared" ref="L6:L11" si="1">-D17</f>
         <v>-0.1</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f t="shared" ref="N6:N11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
+        <f t="shared" ref="N6:N11" si="2">_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
         <v>SRV maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_SRV_MaxGrowth_Biogas</v>
@@ -7549,25 +7780,25 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f t="shared" si="1"/>
-        <v>1.05</v>
+        <f>1+C18</f>
+        <v>1.02</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f t="shared" si="2"/>
-        <v>-0.3</v>
+        <f t="shared" si="1"/>
+        <v>-0.1</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>SRV maximum growth rate of Biogas</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_SRV_MaxGrowth_AmbientHeat</v>
@@ -7589,28 +7820,28 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f t="shared" si="1"/>
-        <v>1.05</v>
+        <f>1+C19</f>
+        <v>1.08</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.3</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>SRV maximum growth rate of AmbientHeat</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A17,"MaxGrowth",B17)</f>
-        <v>*UC_SRV_MaxGrowth_DistrictHeat</v>
+        <f t="shared" si="0"/>
+        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>144</v>
@@ -7629,25 +7860,24 @@
         <v>15</v>
       </c>
       <c r="J9" s="29">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
       </c>
       <c r="L9" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>-0.3</v>
       </c>
       <c r="M9" s="2">
         <v>5</v>
       </c>
       <c r="N9" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>SRV maximum growth rate of DistrictHeat</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_SRV_MaxGrowth_Gas</v>
@@ -7669,25 +7899,25 @@
         <v>15</v>
       </c>
       <c r="J10" s="29">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <f>1+C21</f>
+        <v>1.0149999999999999</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
       </c>
       <c r="L10" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M10" s="2">
         <v>5</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>SRV maximum growth rate of Gas</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_SRV_MaxGrowth_Electricity</v>
@@ -7709,72 +7939,163 @@
         <v>15</v>
       </c>
       <c r="J11" s="29">
-        <f t="shared" si="1"/>
-        <v>1.05</v>
+        <f>1+C22</f>
+        <v>1.08</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
       </c>
       <c r="L11" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.3</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>SRV maximum growth rate of Electricity</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
+        <v>UC_SRV_MaxGrowth_Solar</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="F12" t="s">
+        <v>228</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="29">
+        <f>1+C23</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="16">
+        <f>-D23</f>
+        <v>-0.2</v>
+      </c>
+      <c r="M12" s="2">
+        <v>5</v>
+      </c>
+      <c r="N12" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
+        <v>SRV maximum growth rate of Solar</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MinGrowth",B23)</f>
+        <v>UC_SRV_MinGrowth_Solar</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="F13" t="s">
+        <v>228</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" s="29">
+        <f>1+C23/10</f>
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="16">
+        <f>-D23</f>
+        <v>-0.2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "minimum growth rate of",B23)</f>
+        <v>SRV minimum growth rate of Solar</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MinGrowth",B24)</f>
+        <v>UC_SRV_MinGrowth_LPG</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="F14" t="s">
+        <v>229</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="29">
+        <f>1+C24</f>
+        <v>1.04</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="16">
+        <f>-D24</f>
+        <v>-0.1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>5</v>
+      </c>
+      <c r="N14" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
+        <v>SRV maximum growth rate of LPG</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>117</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="D14">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D15">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" t="s">
-        <v>190</v>
-      </c>
-      <c r="C16" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D16">
-        <v>0.3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -7782,13 +8103,13 @@
         <v>139</v>
       </c>
       <c r="B17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="11">
-        <v>0</v>
+        <v>137</v>
+      </c>
+      <c r="C17" s="54">
+        <v>0.02</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -7796,13 +8117,13 @@
         <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C18" s="11">
-        <v>5.0000000000000001E-3</v>
+        <v>138</v>
+      </c>
+      <c r="C18" s="54">
+        <v>0.02</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -7810,61 +8131,131 @@
         <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>199</v>
-      </c>
-      <c r="C19" s="11">
-        <v>0.05</v>
+        <v>190</v>
+      </c>
+      <c r="C19" s="54">
+        <v>0.08</v>
       </c>
       <c r="D19">
         <v>0.3</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="D20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" s="54">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
+      <c r="A22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" s="54">
+        <v>0.08</v>
+      </c>
+      <c r="D22">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="54">
+        <v>0.15</v>
+      </c>
+      <c r="D23">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="54">
+        <v>0.04</v>
+      </c>
+      <c r="D24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="H22" s="46"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
+      <c r="H26" s="46"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C27" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D27" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E27" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="48" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+      <c r="F27" s="48" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G23" s="48" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
+      <c r="G27" s="48" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H23" s="49" t="s">
+      <c r="H27" s="49" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
         <v>217</v>
       </c>
-      <c r="E24">
+      <c r="E28">
         <v>2018</v>
       </c>
-      <c r="F24">
+      <c r="F28">
         <v>2222</v>
       </c>
-      <c r="G24">
-        <f>F24</f>
+      <c r="G28">
+        <f>F28</f>
         <v>2222</v>
       </c>
-      <c r="H24" t="str">
+      <c r="H28" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F10)</f>
         <v>SRVBIO,SRVBGS,SRVAHT,SRVAHT2,SRVHET*,SRVGAS</v>
       </c>
@@ -9539,12 +9930,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9759,15 +10147,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9792,10 +10184,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Raise DH upper in SRV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A1EE22-E90C-4E4F-B3BD-2D4E75727A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6972146A-D4EE-497F-B1B5-45666CDE9531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -1268,6 +1268,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1280,7 +1281,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2528,12 +2528,12 @@
       <c r="Z15" s="31"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -2617,11 +2617,11 @@
       <c r="A19" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="39"/>
@@ -2649,11 +2649,11 @@
       <c r="A20" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="39"/>
@@ -2741,11 +2741,11 @@
       <c r="A23" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
@@ -2771,11 +2771,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
@@ -2833,11 +2833,11 @@
       <c r="A26" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="51" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
@@ -2953,11 +2953,11 @@
       <c r="A30" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="42"/>
       <c r="F30" s="42"/>
       <c r="G30" s="31"/>
@@ -2985,11 +2985,11 @@
       <c r="A31" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="42"/>
       <c r="F31" s="42"/>
       <c r="G31" s="31"/>
@@ -7606,7 +7606,7 @@
   <dimension ref="A2:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7860,7 +7860,8 @@
         <v>15</v>
       </c>
       <c r="J9" s="29">
-        <v>1.1000000000000001</v>
+        <f>1+C20</f>
+        <v>1.2</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
@@ -8105,7 +8106,7 @@
       <c r="B17" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="50">
         <v>0.02</v>
       </c>
       <c r="D17">
@@ -8119,7 +8120,7 @@
       <c r="B18" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="50">
         <v>0.02</v>
       </c>
       <c r="D18">
@@ -8133,7 +8134,7 @@
       <c r="B19" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="50">
         <v>0.08</v>
       </c>
       <c r="D19">
@@ -8147,8 +8148,8 @@
       <c r="B20" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="54">
-        <v>0.1</v>
+      <c r="C20" s="50">
+        <v>0.2</v>
       </c>
       <c r="D20">
         <v>0.3</v>
@@ -8161,7 +8162,7 @@
       <c r="B21" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="50">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D21">
@@ -8175,7 +8176,7 @@
       <c r="B22" t="s">
         <v>199</v>
       </c>
-      <c r="C22" s="54">
+      <c r="C22" s="50">
         <v>0.08</v>
       </c>
       <c r="D22">
@@ -8189,7 +8190,7 @@
       <c r="B23" t="s">
         <v>203</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C23" s="50">
         <v>0.15</v>
       </c>
       <c r="D23">
@@ -8203,7 +8204,7 @@
       <c r="B24" t="s">
         <v>201</v>
       </c>
-      <c r="C24" s="54">
+      <c r="C24" s="50">
         <v>0.04</v>
       </c>
       <c r="D24">
@@ -9199,7 +9200,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="54" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -9229,7 +9230,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="A31" s="54"/>
       <c r="B31" t="s">
         <v>25</v>
       </c>
@@ -9257,7 +9258,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
+      <c r="A32" s="54"/>
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -9285,7 +9286,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
+      <c r="A33" s="54"/>
       <c r="B33" t="s">
         <v>23</v>
       </c>
@@ -9313,7 +9314,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
+      <c r="A34" s="54"/>
       <c r="B34" t="s">
         <v>22</v>
       </c>
@@ -9341,7 +9342,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
+      <c r="A35" s="54"/>
       <c r="B35" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
DH min 3% grw
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37213EB6-E917-49B3-8399-094E2B0CE11C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5552AE7F-2691-43CC-AE46-F1477688A9B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6580,8 +6580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="J16" s="29">
         <f>1+C32</f>
-        <v>1.06</v>
+        <v>1.03</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
@@ -7454,7 +7454,7 @@
         <v>191</v>
       </c>
       <c r="C32" s="11">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="D32">
         <v>0.3</v>
@@ -9848,6 +9848,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10058,12 +10064,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10074,6 +10074,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10092,15 +10101,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Allign max growth sce
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3042CFA-72F4-4C3A-AF28-780D55A3B3E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832552AC-F698-4AC8-BBF4-110480EFE2F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6581,7 +6581,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6835,7 +6835,7 @@
       </c>
       <c r="J9" s="29">
         <f>1+C27</f>
-        <v>1.1499999999999999</v>
+        <v>1.01</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
@@ -6874,7 +6874,7 @@
         <v>185</v>
       </c>
       <c r="J10" s="29">
-        <f>1-C27*2</f>
+        <f>1-C27*30</f>
         <v>0.7</v>
       </c>
       <c r="K10" s="2">
@@ -6915,7 +6915,7 @@
       </c>
       <c r="J11" s="29">
         <f>1+C28</f>
-        <v>1.1499999999999999</v>
+        <v>1.01</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
@@ -6954,7 +6954,7 @@
         <v>185</v>
       </c>
       <c r="J12" s="29">
-        <f>1-C28*2</f>
+        <f>1-C28*30</f>
         <v>0.7</v>
       </c>
       <c r="K12" s="2">
@@ -7390,7 +7390,7 @@
         <v>197</v>
       </c>
       <c r="C27" s="11">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="D27">
         <v>0.3</v>
@@ -7404,7 +7404,7 @@
         <v>198</v>
       </c>
       <c r="C28" s="11">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="D28">
         <v>0.3</v>
@@ -9840,6 +9840,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10050,15 +10059,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -10066,6 +10066,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10084,14 +10092,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Large Max Growth and minimum DH Plus 4%
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E80BF9-3E1E-4382-9EB0-7004FD28D0F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ADFFF6-F5B3-419C-B2CE-40C72019578B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -5935,7 +5935,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -6580,8 +6580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="J16" s="29">
         <f>1+C32</f>
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
@@ -7460,7 +7460,7 @@
         <v>191</v>
       </c>
       <c r="C32" s="50">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="D32">
         <v>0.3</v>
@@ -8180,8 +8180,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8408,7 +8408,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" si="2"/>
+        <f>-$B$53*L29/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M8" s="2">
@@ -9840,15 +9840,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10059,6 +10050,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -10066,14 +10066,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10092,6 +10084,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
DH min growth 8%
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350AA591-65CB-439E-ADEC-2ADA173156F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F6EAB3-07C2-4C9F-8072-35DE2629E5B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -6581,7 +6581,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="J16" s="29">
         <f>1+C32</f>
-        <v>1.05</v>
+        <v>1.08</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
@@ -7460,7 +7460,7 @@
         <v>191</v>
       </c>
       <c r="C32" s="50">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D32">
         <v>0.3</v>

</xml_diff>

<commit_message>
Max growth for other Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates_DHPlus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CAD987-1BF9-4D31-A138-65D738DFD5E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C417E00-E477-44B2-8A66-F1FAB6D3B283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="3135" yWindow="-13125" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -6468,8 +6468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6643,14 +6643,14 @@
       </c>
       <c r="J7" s="29">
         <f>1+C22</f>
-        <v>1.02</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f>-D23</f>
-        <v>0</v>
+        <f>-D22</f>
+        <v>-0.2</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
@@ -6683,7 +6683,7 @@
       </c>
       <c r="J8" s="29">
         <f>1+C23</f>
-        <v>1.02</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
@@ -7130,10 +7130,10 @@
         <v>196</v>
       </c>
       <c r="C22" s="50">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D22">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -7144,7 +7144,7 @@
         <v>137</v>
       </c>
       <c r="C23" s="50">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -9608,6 +9608,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9818,22 +9833,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9850,21 +9867,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>